<commit_message>
JavaFx Agent Menu Done ,Network Manager,Store Manager and Client Interface done .
</commit_message>
<xml_diff>
--- a/docs/Sprint-D/SprintD - Assessment.xlsx
+++ b/docs/Sprint-D/SprintD - Assessment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9079e2d29d98ec5b/Ambiente de Trabalho/Rodrick/Ensino Superior/Trabalhos ISEP/APROG/Semana 4/lei-23-s2-1dj-g47/docs/Sprint-D/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Desktop/ProjetoIntegrador/docs/Sprint-D/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="8_{A00E38E3-2313-1740-8012-BCB1DFCF5F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30F53927-7C30-467F-B5FA-675F4EE941AF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86904A97-88F7-4D4E-850E-B4ACD224DA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C9F9D952-C72F-9A4E-AE70-234088236500}"/>
+    <workbookView xWindow="7700" yWindow="6580" windowWidth="19420" windowHeight="10300" xr2:uid="{C9F9D952-C72F-9A4E-AE70-234088236500}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -1531,11 +1531,11 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
@@ -1543,19 +1543,19 @@
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="31" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
@@ -1566,7 +1566,7 @@
       <c r="F3" s="76"/>
       <c r="G3" s="76"/>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1574,7 +1574,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
@@ -1582,7 +1582,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1590,7 +1590,7 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>0</v>
       </c>
@@ -1600,7 +1600,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>1</v>
       </c>
@@ -1610,7 +1610,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>2</v>
       </c>
@@ -1620,7 +1620,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>3</v>
       </c>
@@ -1630,7 +1630,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>4</v>
       </c>
@@ -1640,7 +1640,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>5</v>
       </c>
@@ -1650,13 +1650,13 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
@@ -1668,13 +1668,13 @@
       </c>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
@@ -1682,8 +1682,8 @@
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="18" spans="2:20" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:20" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="E18" s="77" t="s">
@@ -1705,7 +1705,7 @@
       <c r="S18" s="78"/>
       <c r="T18" s="79"/>
     </row>
-    <row r="19" spans="2:20" ht="106" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:20" ht="106" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="13">
@@ -1769,7 +1769,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="80" t="s">
         <v>17</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="21" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="81"/>
       <c r="C21" s="21">
         <v>1220917</v>
@@ -1831,16 +1831,26 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="81"/>
       <c r="C22" s="21">
         <v>1220741</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="21"/>
+      <c r="D22" s="21">
+        <v>4</v>
+      </c>
+      <c r="E22" s="22">
+        <v>3</v>
+      </c>
+      <c r="F22" s="17">
+        <v>4</v>
+      </c>
+      <c r="G22" s="23">
+        <v>2</v>
+      </c>
+      <c r="H22" s="21">
+        <v>0</v>
+      </c>
       <c r="I22" s="21"/>
       <c r="J22" s="21"/>
       <c r="K22" s="21"/>
@@ -1851,12 +1861,12 @@
       <c r="P22" s="21"/>
       <c r="Q22" s="21"/>
       <c r="R22" s="24"/>
-      <c r="S22" s="25" t="e">
+      <c r="S22" s="25">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="23" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="81"/>
       <c r="C23" s="21">
         <v>1211221</v>
@@ -1881,7 +1891,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="81"/>
       <c r="C24" s="21">
         <v>1220928</v>
@@ -1906,7 +1916,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="81"/>
       <c r="C25" s="21" t="s">
         <v>18</v>
@@ -1931,7 +1941,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="81"/>
       <c r="C26" s="21" t="s">
         <v>19</v>
@@ -1956,7 +1966,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="81"/>
       <c r="C27" s="21" t="s">
         <v>20</v>
@@ -1981,7 +1991,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="81"/>
       <c r="C28" s="21" t="s">
         <v>21</v>
@@ -2006,7 +2016,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="81"/>
       <c r="C29" s="21" t="s">
         <v>22</v>
@@ -2031,7 +2041,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="81"/>
       <c r="C30" s="21" t="s">
         <v>23</v>
@@ -2056,7 +2066,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="81"/>
       <c r="C31" s="21" t="s">
         <v>24</v>
@@ -2081,7 +2091,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="81"/>
       <c r="C32" s="21" t="s">
         <v>25</v>
@@ -2106,7 +2116,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="81"/>
       <c r="C33" s="21" t="s">
         <v>26</v>
@@ -2131,7 +2141,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="82"/>
       <c r="C34" s="27" t="s">
         <v>27</v>
@@ -2156,7 +2166,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="12" t="s">
         <v>16</v>
@@ -2167,7 +2177,7 @@
       </c>
       <c r="E35" s="31">
         <f t="shared" ref="E35:R35" si="1">AVERAGE(E20:E34)</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="F35" s="31">
         <f t="shared" si="1"/>
@@ -2175,7 +2185,7 @@
       </c>
       <c r="G35" s="31">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H35" s="31">
         <f t="shared" si="1"/>
@@ -2223,10 +2233,10 @@
       </c>
       <c r="S35" s="33"/>
     </row>
-    <row r="37" spans="1:19" ht="31" x14ac:dyDescent="0.7">
+    <row r="37" spans="1:19" ht="31" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="34"/>
     </row>
   </sheetData>
@@ -2255,7 +2265,7 @@
       <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="11" style="73"/>
     <col min="4" max="23" width="7.1640625" style="74" customWidth="1"/>
@@ -2267,7 +2277,7 @@
     <col min="30" max="16384" width="11" style="74"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="40" customFormat="1" ht="344" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" s="40" customFormat="1" ht="344" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="35"/>
       <c r="B1" s="36"/>
       <c r="C1" s="35"/>
@@ -2348,7 +2358,7 @@
       </c>
       <c r="AC1" s="39"/>
     </row>
-    <row r="2" spans="1:29" s="40" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:29" s="40" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>51</v>
       </c>
@@ -2437,7 +2447,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="83" t="s">
         <v>62</v>
       </c>
@@ -2516,7 +2526,7 @@
       <c r="AB3" s="53"/>
       <c r="AC3" s="54"/>
     </row>
-    <row r="4" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="84"/>
       <c r="B4" s="84"/>
       <c r="C4" s="55">
@@ -2558,7 +2568,7 @@
       <c r="AB4" s="62"/>
       <c r="AC4" s="63"/>
     </row>
-    <row r="5" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="84"/>
       <c r="B5" s="84"/>
       <c r="C5" s="55">
@@ -2600,7 +2610,7 @@
       <c r="AB5" s="62"/>
       <c r="AC5" s="63"/>
     </row>
-    <row r="6" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="84"/>
       <c r="B6" s="84"/>
       <c r="C6" s="55">
@@ -2642,7 +2652,7 @@
       <c r="AB6" s="62"/>
       <c r="AC6" s="63"/>
     </row>
-    <row r="7" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="84"/>
       <c r="B7" s="84"/>
       <c r="C7" s="55">
@@ -2684,7 +2694,7 @@
       <c r="AB7" s="62"/>
       <c r="AC7" s="63"/>
     </row>
-    <row r="8" spans="1:29" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:29" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="85"/>
       <c r="B8" s="85"/>
       <c r="C8" s="64"/>
@@ -2724,7 +2734,7 @@
       <c r="AB8" s="71"/>
       <c r="AC8" s="72"/>
     </row>
-    <row r="10" spans="1:29" ht="31" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:29" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
@@ -2735,7 +2745,7 @@
       <c r="F10"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:29" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>60</v>
       </c>
@@ -2746,7 +2756,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:29" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>61</v>
       </c>
@@ -2757,7 +2767,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:29" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>0</v>
       </c>
@@ -2770,7 +2780,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:29" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>1</v>
       </c>
@@ -2783,7 +2793,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:29" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>2</v>
       </c>
@@ -2796,7 +2806,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:29" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>3</v>
       </c>
@@ -2809,7 +2819,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>4</v>
       </c>
@@ -2822,7 +2832,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>5</v>
       </c>
@@ -2861,17 +2871,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="6fb2d6cf-5937-415c-8e29-0a2ba0894026" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40f68083-8b1e-401a-aff0-261d16eabb01">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C8B18F131359BB48BCDE011E677140C8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b731c80a06690715a612fe5879a7430b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40f68083-8b1e-401a-aff0-261d16eabb01" xmlns:ns3="6fb2d6cf-5937-415c-8e29-0a2ba0894026" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="da27ad576f4194a8f5573e372e38eb57" ns2:_="" ns3:_="">
     <xsd:import namespace="40f68083-8b1e-401a-aff0-261d16eabb01"/>
@@ -3088,6 +3087,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6fb2d6cf-5937-415c-8e29-0a2ba0894026" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40f68083-8b1e-401a-aff0-261d16eabb01">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{500E29BA-14B8-49D6-A6F7-C9CFB2D16C3A}">
   <ds:schemaRefs>
@@ -3097,23 +3107,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{831D9D0E-7056-4E72-BBA7-B7F29F987FA7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="6fb2d6cf-5937-415c-8e29-0a2ba0894026"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="40f68083-8b1e-401a-aff0-261d16eabb01"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63DA643D-5E79-43D4-8ED6-24E2F6975D2D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3130,4 +3123,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{831D9D0E-7056-4E72-BBA7-B7F29F987FA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="6fb2d6cf-5937-415c-8e29-0a2ba0894026"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="40f68083-8b1e-401a-aff0-261d16eabb01"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
US17 - documentation completed
</commit_message>
<xml_diff>
--- a/docs/Sprint-D/SprintD - Assessment.xlsx
+++ b/docs/Sprint-D/SprintD - Assessment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Desktop/ProjetoIntegrador/docs/Sprint-D/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leono\Desktop\LEI-1\2º Semestre\ESOFT\2023\LAPR2\docs\Sprint-D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86904A97-88F7-4D4E-850E-B4ACD224DA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C1A9EA-0E6F-4CD6-9A9C-4F39290DD602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7700" yWindow="6580" windowWidth="19420" windowHeight="10300" xr2:uid="{C9F9D952-C72F-9A4E-AE70-234088236500}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C9F9D952-C72F-9A4E-AE70-234088236500}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -1532,30 +1532,30 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="19" width="7.83203125" customWidth="1"/>
+    <col min="4" max="19" width="7.875" customWidth="1"/>
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
@@ -1566,7 +1566,7 @@
       <c r="F3" s="76"/>
       <c r="G3" s="76"/>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1574,7 +1574,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
@@ -1582,7 +1582,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1590,7 +1590,7 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>0</v>
       </c>
@@ -1600,7 +1600,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>1</v>
       </c>
@@ -1610,7 +1610,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>2</v>
       </c>
@@ -1620,7 +1620,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>3</v>
       </c>
@@ -1630,7 +1630,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>4</v>
       </c>
@@ -1640,7 +1640,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>5</v>
       </c>
@@ -1650,13 +1650,13 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
@@ -1668,13 +1668,13 @@
       </c>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
@@ -1682,8 +1682,8 @@
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:20" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:20" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="E18" s="77" t="s">
@@ -1705,7 +1705,7 @@
       <c r="S18" s="78"/>
       <c r="T18" s="79"/>
     </row>
-    <row r="19" spans="2:20" ht="106" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:20" ht="105.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="13">
@@ -1769,7 +1769,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="80" t="s">
         <v>17</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="21" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="81"/>
       <c r="C21" s="21">
         <v>1220917</v>
@@ -1831,7 +1831,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="81"/>
       <c r="C22" s="21">
         <v>1220741</v>
@@ -1866,16 +1866,26 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="23" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="81"/>
       <c r="C23" s="21">
         <v>1211221</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="23"/>
+      <c r="D23" s="21">
+        <v>4</v>
+      </c>
+      <c r="E23" s="21">
+        <v>4</v>
+      </c>
+      <c r="F23" s="22">
+        <v>4</v>
+      </c>
+      <c r="G23" s="17">
+        <v>4</v>
+      </c>
+      <c r="H23" s="23">
+        <v>0</v>
+      </c>
       <c r="I23" s="21"/>
       <c r="J23" s="21"/>
       <c r="K23" s="21"/>
@@ -1886,12 +1896,12 @@
       <c r="P23" s="21"/>
       <c r="Q23" s="21"/>
       <c r="R23" s="24"/>
-      <c r="S23" s="25" t="e">
+      <c r="S23" s="25">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="24" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="81"/>
       <c r="C24" s="21">
         <v>1220928</v>
@@ -1916,7 +1926,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="81"/>
       <c r="C25" s="21" t="s">
         <v>18</v>
@@ -1941,7 +1951,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="81"/>
       <c r="C26" s="21" t="s">
         <v>19</v>
@@ -1966,7 +1976,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="81"/>
       <c r="C27" s="21" t="s">
         <v>20</v>
@@ -1991,7 +2001,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="81"/>
       <c r="C28" s="21" t="s">
         <v>21</v>
@@ -2016,7 +2026,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="81"/>
       <c r="C29" s="21" t="s">
         <v>22</v>
@@ -2041,7 +2051,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="81"/>
       <c r="C30" s="21" t="s">
         <v>23</v>
@@ -2066,7 +2076,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="81"/>
       <c r="C31" s="21" t="s">
         <v>24</v>
@@ -2091,7 +2101,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="81"/>
       <c r="C32" s="21" t="s">
         <v>25</v>
@@ -2116,7 +2126,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="81"/>
       <c r="C33" s="21" t="s">
         <v>26</v>
@@ -2141,7 +2151,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="82"/>
       <c r="C34" s="27" t="s">
         <v>27</v>
@@ -2166,7 +2176,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
       <c r="C35" s="12" t="s">
         <v>16</v>
@@ -2177,7 +2187,7 @@
       </c>
       <c r="E35" s="31">
         <f t="shared" ref="E35:R35" si="1">AVERAGE(E20:E34)</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F35" s="31">
         <f t="shared" si="1"/>
@@ -2185,7 +2195,7 @@
       </c>
       <c r="G35" s="31">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="H35" s="31">
         <f t="shared" si="1"/>
@@ -2233,10 +2243,10 @@
       </c>
       <c r="S35" s="33"/>
     </row>
-    <row r="37" spans="1:19" ht="31" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:19" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A37" s="3"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="34"/>
     </row>
   </sheetData>
@@ -2265,19 +2275,19 @@
       <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="11" style="73"/>
-    <col min="4" max="23" width="7.1640625" style="74" customWidth="1"/>
+    <col min="4" max="23" width="7.125" style="74" customWidth="1"/>
     <col min="24" max="24" width="11" style="74"/>
     <col min="25" max="26" width="11" style="73"/>
     <col min="27" max="27" width="11" style="75"/>
-    <col min="28" max="28" width="13.1640625" style="74" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.125" style="74" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="35" style="74" customWidth="1"/>
     <col min="30" max="16384" width="11" style="74"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="40" customFormat="1" ht="344" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" s="40" customFormat="1" ht="344.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35"/>
       <c r="B1" s="36"/>
       <c r="C1" s="35"/>
@@ -2358,7 +2368,7 @@
       </c>
       <c r="AC1" s="39"/>
     </row>
-    <row r="2" spans="1:29" s="40" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" s="40" customFormat="1" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="41" t="s">
         <v>51</v>
       </c>
@@ -2447,7 +2457,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="83" t="s">
         <v>62</v>
       </c>
@@ -2526,7 +2536,7 @@
       <c r="AB3" s="53"/>
       <c r="AC3" s="54"/>
     </row>
-    <row r="4" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="84"/>
       <c r="B4" s="84"/>
       <c r="C4" s="55">
@@ -2568,7 +2578,7 @@
       <c r="AB4" s="62"/>
       <c r="AC4" s="63"/>
     </row>
-    <row r="5" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="84"/>
       <c r="B5" s="84"/>
       <c r="C5" s="55">
@@ -2610,7 +2620,7 @@
       <c r="AB5" s="62"/>
       <c r="AC5" s="63"/>
     </row>
-    <row r="6" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="84"/>
       <c r="B6" s="84"/>
       <c r="C6" s="55">
@@ -2652,7 +2662,7 @@
       <c r="AB6" s="62"/>
       <c r="AC6" s="63"/>
     </row>
-    <row r="7" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="84"/>
       <c r="B7" s="84"/>
       <c r="C7" s="55">
@@ -2694,7 +2704,7 @@
       <c r="AB7" s="62"/>
       <c r="AC7" s="63"/>
     </row>
-    <row r="8" spans="1:29" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" customFormat="1" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="85"/>
       <c r="B8" s="85"/>
       <c r="C8" s="64"/>
@@ -2734,7 +2744,7 @@
       <c r="AB8" s="71"/>
       <c r="AC8" s="72"/>
     </row>
-    <row r="10" spans="1:29" ht="31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:29" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
@@ -2745,7 +2755,7 @@
       <c r="F10"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:29" ht="19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>60</v>
       </c>
@@ -2756,7 +2766,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:29" ht="19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>61</v>
       </c>
@@ -2767,7 +2777,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:29" ht="19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>0</v>
       </c>
@@ -2780,7 +2790,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:29" ht="19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>1</v>
       </c>
@@ -2793,7 +2803,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:29" ht="19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>2</v>
       </c>
@@ -2806,7 +2816,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:29" ht="19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>3</v>
       </c>
@@ -2819,7 +2829,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>4</v>
       </c>
@@ -2832,7 +2842,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>5</v>
       </c>
@@ -2862,15 +2872,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C8B18F131359BB48BCDE011E677140C8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b731c80a06690715a612fe5879a7430b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40f68083-8b1e-401a-aff0-261d16eabb01" xmlns:ns3="6fb2d6cf-5937-415c-8e29-0a2ba0894026" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="da27ad576f4194a8f5573e372e38eb57" ns2:_="" ns3:_="">
     <xsd:import namespace="40f68083-8b1e-401a-aff0-261d16eabb01"/>
@@ -3087,6 +3088,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3099,14 +3109,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{500E29BA-14B8-49D6-A6F7-C9CFB2D16C3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63DA643D-5E79-43D4-8ED6-24E2F6975D2D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3121,6 +3123,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{500E29BA-14B8-49D6-A6F7-C9CFB2D16C3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
us15 and us16 sd,ssd,cd , md and readme - final alterations addictions on class diagram and on  project domain model
</commit_message>
<xml_diff>
--- a/docs/Sprint-D/SprintD - Assessment.xlsx
+++ b/docs/Sprint-D/SprintD - Assessment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leono\Desktop\LEI-1\2º Semestre\ESOFT\2023\LAPR2\docs\Sprint-D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\OneDrive\Ambiente de Trabalho\submissãoSprintC\docs\Sprint-D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C1A9EA-0E6F-4CD6-9A9C-4F39290DD602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C835D188-935E-4E97-9738-BA7EA53E2497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C9F9D952-C72F-9A4E-AE70-234088236500}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C9F9D952-C72F-9A4E-AE70-234088236500}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -1531,8 +1531,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1811,11 +1811,21 @@
       <c r="C21" s="21">
         <v>1220917</v>
       </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
+      <c r="D21" s="22">
+        <v>4</v>
+      </c>
+      <c r="E21" s="17">
+        <v>3</v>
+      </c>
+      <c r="F21" s="23">
+        <v>4</v>
+      </c>
+      <c r="G21" s="21">
+        <v>3</v>
+      </c>
+      <c r="H21" s="21">
+        <v>0</v>
+      </c>
       <c r="I21" s="21"/>
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
@@ -1826,9 +1836,9 @@
       <c r="P21" s="21"/>
       <c r="Q21" s="21"/>
       <c r="R21" s="24"/>
-      <c r="S21" s="25" t="e">
+      <c r="S21" s="25">
         <f t="shared" ref="S21:S34" si="0">AVERAGE(D21:R21)</f>
-        <v>#DIV/0!</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="22" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2195,7 +2205,7 @@
       </c>
       <c r="G35" s="31">
         <f t="shared" si="1"/>
-        <v>2.3333333333333335</v>
+        <v>2.5</v>
       </c>
       <c r="H35" s="31">
         <f t="shared" si="1"/>
@@ -2872,6 +2882,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6fb2d6cf-5937-415c-8e29-0a2ba0894026" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40f68083-8b1e-401a-aff0-261d16eabb01">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C8B18F131359BB48BCDE011E677140C8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b731c80a06690715a612fe5879a7430b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40f68083-8b1e-401a-aff0-261d16eabb01" xmlns:ns3="6fb2d6cf-5937-415c-8e29-0a2ba0894026" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="da27ad576f4194a8f5573e372e38eb57" ns2:_="" ns3:_="">
     <xsd:import namespace="40f68083-8b1e-401a-aff0-261d16eabb01"/>
@@ -3088,27 +3118,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{831D9D0E-7056-4E72-BBA7-B7F29F987FA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="6fb2d6cf-5937-415c-8e29-0a2ba0894026"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="40f68083-8b1e-401a-aff0-261d16eabb01"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="6fb2d6cf-5937-415c-8e29-0a2ba0894026" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40f68083-8b1e-401a-aff0-261d16eabb01">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{500E29BA-14B8-49D6-A6F7-C9CFB2D16C3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63DA643D-5E79-43D4-8ED6-24E2F6975D2D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3125,29 +3160,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{500E29BA-14B8-49D6-A6F7-C9CFB2D16C3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{831D9D0E-7056-4E72-BBA7-B7F29F987FA7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="6fb2d6cf-5937-415c-8e29-0a2ba0894026"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="40f68083-8b1e-401a-aff0-261d16eabb01"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Esoft final Commit us002 us018
</commit_message>
<xml_diff>
--- a/docs/Sprint-D/SprintD - Assessment.xlsx
+++ b/docs/Sprint-D/SprintD - Assessment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\OneDrive\Ambiente de Trabalho\submissãoSprintC\docs\Sprint-D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Desktop/ProjetoIntegrador/docs/Sprint-D/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C835D188-935E-4E97-9738-BA7EA53E2497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6793A2A8-2BDD-684D-9415-B4E479130BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C9F9D952-C72F-9A4E-AE70-234088236500}"/>
+    <workbookView xWindow="7700" yWindow="6580" windowWidth="19420" windowHeight="10300" xr2:uid="{C9F9D952-C72F-9A4E-AE70-234088236500}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -1531,31 +1531,31 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="19" width="7.875" customWidth="1"/>
+    <col min="4" max="19" width="7.83203125" customWidth="1"/>
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
@@ -1566,7 +1566,7 @@
       <c r="F3" s="76"/>
       <c r="G3" s="76"/>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1574,7 +1574,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
@@ -1582,7 +1582,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1590,7 +1590,7 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>0</v>
       </c>
@@ -1600,7 +1600,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>1</v>
       </c>
@@ -1610,7 +1610,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>2</v>
       </c>
@@ -1620,7 +1620,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>3</v>
       </c>
@@ -1630,7 +1630,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>4</v>
       </c>
@@ -1640,7 +1640,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>5</v>
       </c>
@@ -1650,13 +1650,13 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
@@ -1668,13 +1668,13 @@
       </c>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
@@ -1682,8 +1682,8 @@
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:20" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:20" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="E18" s="77" t="s">
@@ -1705,7 +1705,7 @@
       <c r="S18" s="78"/>
       <c r="T18" s="79"/>
     </row>
-    <row r="19" spans="2:20" ht="105.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:20" ht="106" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="13">
@@ -1769,7 +1769,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="80" t="s">
         <v>17</v>
       </c>
@@ -1806,26 +1806,16 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="21" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="81"/>
       <c r="C21" s="21">
         <v>1220917</v>
       </c>
-      <c r="D21" s="22">
-        <v>4</v>
-      </c>
-      <c r="E21" s="17">
-        <v>3</v>
-      </c>
-      <c r="F21" s="23">
-        <v>4</v>
-      </c>
-      <c r="G21" s="21">
-        <v>3</v>
-      </c>
-      <c r="H21" s="21">
-        <v>0</v>
-      </c>
+      <c r="D21" s="22"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
       <c r="I21" s="21"/>
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
@@ -1836,12 +1826,12 @@
       <c r="P21" s="21"/>
       <c r="Q21" s="21"/>
       <c r="R21" s="24"/>
-      <c r="S21" s="25">
+      <c r="S21" s="25" t="e">
         <f t="shared" ref="S21:S34" si="0">AVERAGE(D21:R21)</f>
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="22" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="81"/>
       <c r="C22" s="21">
         <v>1220741</v>
@@ -1856,7 +1846,7 @@
         <v>4</v>
       </c>
       <c r="G22" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H22" s="21">
         <v>0</v>
@@ -1873,29 +1863,19 @@
       <c r="R22" s="24"/>
       <c r="S22" s="25">
         <f t="shared" si="0"/>
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="23" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="81"/>
       <c r="C23" s="21">
         <v>1211221</v>
       </c>
-      <c r="D23" s="21">
-        <v>4</v>
-      </c>
-      <c r="E23" s="21">
-        <v>4</v>
-      </c>
-      <c r="F23" s="22">
-        <v>4</v>
-      </c>
-      <c r="G23" s="17">
-        <v>4</v>
-      </c>
-      <c r="H23" s="23">
-        <v>0</v>
-      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="23"/>
       <c r="I23" s="21"/>
       <c r="J23" s="21"/>
       <c r="K23" s="21"/>
@@ -1906,12 +1886,12 @@
       <c r="P23" s="21"/>
       <c r="Q23" s="21"/>
       <c r="R23" s="24"/>
-      <c r="S23" s="25">
+      <c r="S23" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="81"/>
       <c r="C24" s="21">
         <v>1220928</v>
@@ -1936,7 +1916,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="81"/>
       <c r="C25" s="21" t="s">
         <v>18</v>
@@ -1961,7 +1941,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="81"/>
       <c r="C26" s="21" t="s">
         <v>19</v>
@@ -1986,7 +1966,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="81"/>
       <c r="C27" s="21" t="s">
         <v>20</v>
@@ -2011,7 +1991,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="81"/>
       <c r="C28" s="21" t="s">
         <v>21</v>
@@ -2036,7 +2016,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="81"/>
       <c r="C29" s="21" t="s">
         <v>22</v>
@@ -2061,7 +2041,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="81"/>
       <c r="C30" s="21" t="s">
         <v>23</v>
@@ -2086,7 +2066,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="81"/>
       <c r="C31" s="21" t="s">
         <v>24</v>
@@ -2111,7 +2091,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="81"/>
       <c r="C32" s="21" t="s">
         <v>25</v>
@@ -2136,7 +2116,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="81"/>
       <c r="C33" s="21" t="s">
         <v>26</v>
@@ -2161,7 +2141,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="82"/>
       <c r="C34" s="27" t="s">
         <v>27</v>
@@ -2186,7 +2166,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="12" t="s">
         <v>16</v>
@@ -2197,7 +2177,7 @@
       </c>
       <c r="E35" s="31">
         <f t="shared" ref="E35:R35" si="1">AVERAGE(E20:E34)</f>
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="F35" s="31">
         <f t="shared" si="1"/>
@@ -2205,7 +2185,7 @@
       </c>
       <c r="G35" s="31">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="H35" s="31">
         <f t="shared" si="1"/>
@@ -2253,10 +2233,10 @@
       </c>
       <c r="S35" s="33"/>
     </row>
-    <row r="37" spans="1:19" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:19" ht="31" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="34"/>
     </row>
   </sheetData>
@@ -2285,19 +2265,19 @@
       <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="11" style="73"/>
-    <col min="4" max="23" width="7.125" style="74" customWidth="1"/>
+    <col min="4" max="23" width="7.1640625" style="74" customWidth="1"/>
     <col min="24" max="24" width="11" style="74"/>
     <col min="25" max="26" width="11" style="73"/>
     <col min="27" max="27" width="11" style="75"/>
-    <col min="28" max="28" width="13.125" style="74" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.1640625" style="74" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="35" style="74" customWidth="1"/>
     <col min="30" max="16384" width="11" style="74"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="40" customFormat="1" ht="344.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" s="40" customFormat="1" ht="344" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="35"/>
       <c r="B1" s="36"/>
       <c r="C1" s="35"/>
@@ -2378,7 +2358,7 @@
       </c>
       <c r="AC1" s="39"/>
     </row>
-    <row r="2" spans="1:29" s="40" customFormat="1" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" s="40" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>51</v>
       </c>
@@ -2467,7 +2447,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:29" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="83" t="s">
         <v>62</v>
       </c>
@@ -2546,7 +2526,7 @@
       <c r="AB3" s="53"/>
       <c r="AC3" s="54"/>
     </row>
-    <row r="4" spans="1:29" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="84"/>
       <c r="B4" s="84"/>
       <c r="C4" s="55">
@@ -2588,7 +2568,7 @@
       <c r="AB4" s="62"/>
       <c r="AC4" s="63"/>
     </row>
-    <row r="5" spans="1:29" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="84"/>
       <c r="B5" s="84"/>
       <c r="C5" s="55">
@@ -2630,7 +2610,7 @@
       <c r="AB5" s="62"/>
       <c r="AC5" s="63"/>
     </row>
-    <row r="6" spans="1:29" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="84"/>
       <c r="B6" s="84"/>
       <c r="C6" s="55">
@@ -2672,7 +2652,7 @@
       <c r="AB6" s="62"/>
       <c r="AC6" s="63"/>
     </row>
-    <row r="7" spans="1:29" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="84"/>
       <c r="B7" s="84"/>
       <c r="C7" s="55">
@@ -2714,7 +2694,7 @@
       <c r="AB7" s="62"/>
       <c r="AC7" s="63"/>
     </row>
-    <row r="8" spans="1:29" customFormat="1" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="85"/>
       <c r="B8" s="85"/>
       <c r="C8" s="64"/>
@@ -2754,7 +2734,7 @@
       <c r="AB8" s="71"/>
       <c r="AC8" s="72"/>
     </row>
-    <row r="10" spans="1:29" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:29" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
@@ -2765,7 +2745,7 @@
       <c r="F10"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>60</v>
       </c>
@@ -2776,7 +2756,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>61</v>
       </c>
@@ -2787,7 +2767,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>0</v>
       </c>
@@ -2800,7 +2780,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>1</v>
       </c>
@@ -2813,7 +2793,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>2</v>
       </c>
@@ -2826,7 +2806,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>3</v>
       </c>
@@ -2839,7 +2819,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>4</v>
       </c>
@@ -2852,7 +2832,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>5</v>
       </c>
@@ -2882,6 +2862,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="6fb2d6cf-5937-415c-8e29-0a2ba0894026" xsi:nil="true"/>
@@ -2890,15 +2879,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3119,6 +3099,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{500E29BA-14B8-49D6-A6F7-C9CFB2D16C3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{831D9D0E-7056-4E72-BBA7-B7F29F987FA7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -3131,14 +3119,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{500E29BA-14B8-49D6-A6F7-C9CFB2D16C3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>